<commit_message>
add: nueva versión de la guía 0.1.3
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-CSEstablecimientoDestinoCodigo.xlsx
+++ b/docs/CodeSystem-CSEstablecimientoDestinoCodigo.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.2</t>
+    <t>0.1.3</t>
   </si>
   <si>
     <t>Name</t>
@@ -159,19 +159,19 @@
     <t>101203</t>
   </si>
   <si>
-    <t xml:space="preserve">SEREMI De Arica y Parinacota Clínica Hebe </t>
+    <t>SEREMI De Arica y Parinacota Clínica Hebe</t>
   </si>
   <si>
     <t>101212</t>
   </si>
   <si>
-    <t xml:space="preserve">SEREMI De Arica y Parinacota Clínica San Agustín </t>
+    <t>SEREMI De Arica y Parinacota Clínica San Agustín</t>
   </si>
   <si>
     <t>101213</t>
   </si>
   <si>
-    <t xml:space="preserve">SEREMI De Arica y Parinacota Clínica San José </t>
+    <t>SEREMI De Arica y Parinacota Clínica San José</t>
   </si>
   <si>
     <t>101214</t>
@@ -183,7 +183,7 @@
     <t>101215</t>
   </si>
   <si>
-    <t xml:space="preserve">SEREMI De Arica y Parinacota Complejo Penitenciario </t>
+    <t>SEREMI De Arica y Parinacota Complejo Penitenciario</t>
   </si>
   <si>
     <t>101216</t>

</xml_diff>